<commit_message>
Good version run 2 DAC and 1 ADC
</commit_message>
<xml_diff>
--- a/algorithm/testbench/pcmmux.xlsx
+++ b/algorithm/testbench/pcmmux.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chenyu\RTL_work\RTL_work\UltraSound\algorithm\testbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E0B68-0FCE-4177-A1C4-0BC0E800951A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C6B926-76C6-481C-9560-AF0E084A1FAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2026168C-CC0B-4042-8725-47D1C9FEE1DA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>wr_addr</t>
   </si>
@@ -124,6 +124,48 @@
   </si>
   <si>
     <t>valid_p</t>
+  </si>
+  <si>
+    <t>pcmaw=1</t>
+  </si>
+  <si>
+    <t>pcmaw&gt;1</t>
+  </si>
+  <si>
+    <t>pcm_in_valid</t>
+  </si>
+  <si>
+    <t>pcm</t>
+  </si>
+  <si>
+    <t>phase0</t>
+  </si>
+  <si>
+    <t>phase1</t>
+  </si>
+  <si>
+    <t>phase2</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>Q0</t>
+  </si>
+  <si>
+    <t>mult_result</t>
+  </si>
+  <si>
+    <t>ipcm_out</t>
+  </si>
+  <si>
+    <t>qpcm_out</t>
+  </si>
+  <si>
+    <t>I0_32</t>
+  </si>
+  <si>
+    <t>Q0_32</t>
   </si>
 </sst>
 </file>
@@ -185,6 +227,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CAD26E3-6F2E-4977-81A3-D94CAEB0D55B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="838200" y="13898880"/>
+          <a:ext cx="1226820" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,15 +592,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132DC023-D26D-41D3-AACB-137C2BB7D6ED}">
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:S120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,6 +926,11 @@
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>1F0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1724,7 +1837,9 @@
       <c r="S59" s="1"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2190,13 +2305,19 @@
       <c r="P73" s="1"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="G74" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -2208,13 +2329,27 @@
       <c r="P74" s="1"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <v>1</v>
+      </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -2226,14 +2361,26 @@
       <c r="P75" s="1"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
@@ -2244,14 +2391,30 @@
       <c r="P76" s="1"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
@@ -2262,14 +2425,30 @@
       <c r="P77" s="1"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
@@ -2280,12 +2459,18 @@
       <c r="P78" s="1"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="E79" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -2298,12 +2483,16 @@
       <c r="P79" s="1"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -2316,13 +2505,17 @@
       <c r="P80" s="1"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
+      <c r="A81" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="G81" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2369,9 +2562,602 @@
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
     </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>